<commit_message>
Output quoted strings into excel file
</commit_message>
<xml_diff>
--- a/testcode/excel/excel_files/testing.xlsx
+++ b/testcode/excel/excel_files/testing.xlsx
@@ -14,9 +14,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
-  <si>
-    <t>Hi Excel!</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>sampletext</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>There</t>
+  </si>
+  <si>
+    <t>illegal</t>
+  </si>
+  <si>
+    <t>will fail</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>generate</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>legal</t>
   </si>
 </sst>
 </file>
@@ -359,31 +383,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3">
-        <v>1.2345</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4">
-        <f>SIN(PI()/4)</f>
-        <v>0</v>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>